<commit_message>
exporting all the category xlsx
</commit_message>
<xml_diff>
--- a/electron/templates/Stocks.xlsx
+++ b/electron/templates/Stocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8D52FE-0F53-42C6-BB45-3D73B1B8C972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848A4189-5ECC-44E2-8469-C209EE7B4680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="121">
   <si>
     <t>Order Block</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>Sentiment Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMI	</t>
   </si>
 </sst>
 </file>
@@ -934,7 +937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -963,72 +966,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1038,6 +981,93 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
     </xf>
@@ -1050,58 +1080,64 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1113,50 +1149,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1440,7 +1440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="126" workbookViewId="0">
+    <sheetView zoomScale="126" workbookViewId="0">
       <selection activeCell="C54" activeCellId="1" sqref="I48 C54"/>
     </sheetView>
   </sheetViews>
@@ -1480,33 +1480,33 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="47" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="21" t="s">
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="21" t="s">
+      <c r="G2" s="24"/>
+      <c r="H2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="23"/>
+      <c r="I2" s="25"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
-      <c r="B3" s="39"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1532,11 +1532,11 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="3"/>
@@ -1549,9 +1549,9 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="30" t="s">
+      <c r="A5" s="45"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="3"/>
@@ -1564,9 +1564,9 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="30" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3"/>
@@ -1579,9 +1579,9 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="30" t="s">
+      <c r="A7" s="45"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="3"/>
@@ -1594,9 +1594,9 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="30" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="3"/>
@@ -1609,9 +1609,9 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="30" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="3"/>
@@ -1624,9 +1624,9 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="32" t="s">
+      <c r="A10" s="45"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="12" t="s">
         <v>81</v>
       </c>
       <c r="D10" s="3"/>
@@ -1639,9 +1639,9 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="32" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="3"/>
@@ -1654,9 +1654,9 @@
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="33" t="s">
+      <c r="A12" s="45"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="3"/>
@@ -1669,9 +1669,9 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="34" t="s">
+      <c r="A13" s="45"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="14" t="s">
         <v>79</v>
       </c>
       <c r="D13" s="3"/>
@@ -1684,9 +1684,9 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="30" t="s">
+      <c r="A14" s="45"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="3"/>
@@ -1699,9 +1699,9 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="30" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="3"/>
@@ -1714,9 +1714,9 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="30" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="3"/>
@@ -1729,9 +1729,9 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="30" t="s">
+      <c r="A17" s="45"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="3"/>
@@ -1744,9 +1744,9 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="30" t="s">
+      <c r="A18" s="45"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="3"/>
@@ -1759,9 +1759,9 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="32" t="s">
+      <c r="A19" s="45"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="12" t="s">
         <v>80</v>
       </c>
       <c r="D19" s="3"/>
@@ -1774,9 +1774,9 @@
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="30" t="s">
+      <c r="A20" s="45"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="3"/>
@@ -1789,9 +1789,9 @@
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="30" t="s">
+      <c r="A21" s="45"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="3"/>
@@ -1804,9 +1804,9 @@
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="30" t="s">
+      <c r="A22" s="45"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="3"/>
@@ -1819,9 +1819,9 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="30" t="s">
+      <c r="A23" s="45"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="3"/>
@@ -1834,9 +1834,9 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="30" t="s">
+      <c r="A24" s="45"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="3"/>
@@ -1848,10 +1848,10 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="30" t="s">
+    <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="45"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="3"/>
@@ -1864,9 +1864,9 @@
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="30" t="s">
+      <c r="A26" s="45"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="3"/>
@@ -1879,9 +1879,9 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="36"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="30" t="s">
+      <c r="A27" s="45"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="3"/>
@@ -1894,9 +1894,9 @@
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="30" t="s">
+      <c r="A28" s="45"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D28" s="3"/>
@@ -1909,9 +1909,9 @@
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="36"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="30" t="s">
+      <c r="A29" s="45"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D29" s="3"/>
@@ -1924,9 +1924,9 @@
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="36"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="30" t="s">
+      <c r="A30" s="45"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D30" s="3"/>
@@ -1939,9 +1939,9 @@
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="36"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="30" t="s">
+      <c r="A31" s="45"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="11" t="s">
         <v>34</v>
       </c>
       <c r="D31" s="3"/>
@@ -1954,9 +1954,9 @@
       <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="36"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="30" t="s">
+      <c r="A32" s="45"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D32" s="3"/>
@@ -1969,9 +1969,9 @@
       <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="30" t="s">
+      <c r="A33" s="45"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="11" t="s">
         <v>36</v>
       </c>
       <c r="D33" s="3"/>
@@ -1984,9 +1984,9 @@
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A34" s="36"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="30" t="s">
+      <c r="A34" s="45"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D34" s="3"/>
@@ -1999,9 +1999,9 @@
       <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A35" s="36"/>
-      <c r="B35" s="41"/>
-      <c r="C35" s="30" t="s">
+      <c r="A35" s="45"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D35" s="3"/>
@@ -2014,9 +2014,9 @@
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A36" s="36"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="30" t="s">
+      <c r="A36" s="45"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D36" s="3"/>
@@ -2029,9 +2029,9 @@
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A37" s="36"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="30" t="s">
+      <c r="A37" s="45"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="11" t="s">
         <v>40</v>
       </c>
       <c r="D37" s="3"/>
@@ -2044,9 +2044,9 @@
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A38" s="36"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="30" t="s">
+      <c r="A38" s="45"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D38" s="3"/>
@@ -2059,8 +2059,8 @@
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A39" s="36"/>
-      <c r="B39" s="43" t="s">
+      <c r="A39" s="45"/>
+      <c r="B39" s="29" t="s">
         <v>48</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -2088,8 +2088,8 @@
       <c r="W39" s="1"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A40" s="36"/>
-      <c r="B40" s="44"/>
+      <c r="A40" s="45"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="5" t="s">
         <v>43</v>
       </c>
@@ -2115,8 +2115,8 @@
       <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A41" s="36"/>
-      <c r="B41" s="44"/>
+      <c r="A41" s="45"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="5" t="s">
         <v>44</v>
       </c>
@@ -2142,8 +2142,8 @@
       <c r="W41" s="1"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A42" s="36"/>
-      <c r="B42" s="39"/>
+      <c r="A42" s="45"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="5" t="s">
         <v>45</v>
       </c>
@@ -2169,17 +2169,17 @@
       <c r="W42" s="1"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A43" s="36"/>
-      <c r="B43" s="45" t="s">
+      <c r="A43" s="45"/>
+      <c r="B43" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="12"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="37"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -2196,15 +2196,15 @@
       <c r="W43" s="1"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A44" s="36"/>
-      <c r="B44" s="46"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="14"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="40"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -2221,15 +2221,15 @@
       <c r="W44" s="1"/>
     </row>
     <row r="45" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="37"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="17"/>
+      <c r="A45" s="46"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="43"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -2324,15 +2324,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:I45"/>
+    <mergeCell ref="A2:A45"/>
+    <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="B4:B38"/>
     <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:I45"/>
-    <mergeCell ref="A2:A45"/>
-    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2341,10 +2341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8DA3849-4350-404B-AA0C-798A91D6185C}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2362,246 +2362,246 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="21" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="23"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
-      <c r="B2" s="57" t="s">
+      <c r="A2" s="52"/>
+      <c r="B2" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="50"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="19" t="s">
+      <c r="A3" s="52"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="50"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="56"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="64"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="19" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="50"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="56"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="64"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="19" t="s">
+      <c r="A5" s="52"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="50"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="56"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="64"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="19" t="s">
+      <c r="A6" s="52"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="50"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="56"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="64"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="52"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="50"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="56"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="64"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="19" t="s">
+      <c r="A8" s="52"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="50"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="64"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="19" t="s">
+      <c r="A9" s="52"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="50"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="56"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="64"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="19" t="s">
+      <c r="A10" s="52"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="50"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="56"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="64"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="19" t="s">
+      <c r="A11" s="52"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="50"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="56"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="64"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="19" t="s">
+      <c r="A12" s="52"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="50"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="56"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="64"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="19" t="s">
+      <c r="A13" s="52"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="50"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="56"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="64"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="19" t="s">
+      <c r="A14" s="52"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="50"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="56"/>
     </row>
     <row r="15" spans="1:12" ht="24" x14ac:dyDescent="0.3">
-      <c r="A15" s="64"/>
-      <c r="B15" s="60" t="s">
+      <c r="A15" s="52"/>
+      <c r="B15" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="31"/>
+      <c r="D15" s="66"/>
       <c r="E15" s="6" t="s">
         <v>71</v>
       </c>
@@ -2623,17 +2623,17 @@
       <c r="K15" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="L15" s="66" t="s">
+      <c r="L15" s="18" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="64"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="18" t="s">
+      <c r="A16" s="52"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="31"/>
+      <c r="D16" s="66"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -2644,12 +2644,12 @@
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="18" t="s">
+      <c r="A17" s="52"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="31"/>
+      <c r="D17" s="66"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -2660,12 +2660,12 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="64"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="18" t="s">
+      <c r="A18" s="52"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="31"/>
+      <c r="D18" s="66"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -2676,12 +2676,12 @@
       <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="64"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="18" t="s">
+      <c r="A19" s="52"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="31"/>
+      <c r="D19" s="66"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -2692,12 +2692,12 @@
       <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="64"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="18" t="s">
+      <c r="A20" s="52"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="31"/>
+      <c r="D20" s="66"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -2708,12 +2708,12 @@
       <c r="L20" s="7"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="64"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="31"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="66"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -2724,12 +2724,12 @@
       <c r="L21" s="7"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="64"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="31"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="66"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -2740,12 +2740,12 @@
       <c r="L22" s="7"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="64"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="31"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="66"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -2756,12 +2756,12 @@
       <c r="L23" s="7"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="64"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="31"/>
+      <c r="A24" s="52"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="66"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -2772,12 +2772,12 @@
       <c r="L24" s="7"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="64"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="31"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="66"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -2788,12 +2788,12 @@
       <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="64"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="31"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="65" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="66"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -2803,251 +2803,215 @@
       <c r="K26" s="6"/>
       <c r="L26" s="7"/>
     </row>
-    <row r="27" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="64"/>
-      <c r="B27" s="29" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="52"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="66"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="7"/>
+    </row>
+    <row r="28" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="52"/>
+      <c r="B28" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C28" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="50"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="64"/>
-      <c r="B28" s="26" t="s">
+      <c r="D28" s="57"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="56"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="52"/>
+      <c r="B29" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C29" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="19" t="s">
+      <c r="D29" s="57"/>
+      <c r="E29" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="19" t="s">
+      <c r="F29" s="57"/>
+      <c r="G29" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="19" t="s">
+      <c r="H29" s="55"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="K28" s="20"/>
-      <c r="L28" s="50"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="64"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="19" t="s">
+      <c r="K29" s="55"/>
+      <c r="L29" s="56"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="52"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="50"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="64"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="57"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="55"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="56"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="52"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="50"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="64"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="19" t="s">
+      <c r="D31" s="57"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="56"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="52"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="50"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="64"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="19" t="s">
+      <c r="D32" s="57"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="55"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="55"/>
+      <c r="L32" s="56"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="52"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="50"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="64"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="19" t="s">
+      <c r="D33" s="57"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="56"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="52"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="50"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="64"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="19" t="s">
+      <c r="D34" s="57"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="57"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="56"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="52"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="50"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="64"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="19" t="s">
+      <c r="D35" s="57"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="57"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="56"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="52"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="50"/>
-    </row>
-    <row r="36" spans="1:12" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="65"/>
-      <c r="B36" s="51" t="s">
+      <c r="D36" s="57"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="56"/>
+    </row>
+    <row r="37" spans="1:12" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="53"/>
+      <c r="B37" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C37" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="53"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="55"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="104">
-    <mergeCell ref="E36:L36"/>
-    <mergeCell ref="A1:A36"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E35:L35"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B15:B26"/>
-    <mergeCell ref="E27:L27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="B28:B35"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:L9"/>
+  <mergeCells count="105">
+    <mergeCell ref="B2:B14"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J3:L3"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="J6:L6"/>
@@ -3062,25 +3026,78 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="J5:L5"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E1:L1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="B2:B14"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B15:B27"/>
+    <mergeCell ref="E28:L28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="B29:B36"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E37:L37"/>
+    <mergeCell ref="A1:A37"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E36:L36"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3089,7 +3106,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018BC9BF-F888-4B54-8F04-0551ED1224D4}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -3097,136 +3114,125 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="68"/>
-    <col min="2" max="2" width="27.21875" style="68" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="68"/>
+    <col min="1" max="1" width="8.88671875" style="19"/>
+    <col min="2" max="2" width="27.21875" style="19" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="71"/>
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="72"/>
       <c r="B3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="72"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="72"/>
       <c r="B4" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="72"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="71"/>
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="72"/>
       <c r="B5" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="72"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="71"/>
+      <c r="C5" s="21"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="72"/>
       <c r="B6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="72"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="71"/>
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="72"/>
       <c r="B7" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="72"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="71"/>
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="72"/>
       <c r="B8" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="72"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="71"/>
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="72"/>
       <c r="B9" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="72"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="71"/>
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="72"/>
       <c r="B10" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="72"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="71"/>
+      <c r="C10" s="21"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="72"/>
       <c r="B11" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="72"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="72"/>
       <c r="B12" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="72"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="71"/>
+      <c r="C12" s="21"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="72"/>
       <c r="B13" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="72"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="71"/>
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="72"/>
       <c r="B14" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C14" s="72"/>
-    </row>
-    <row r="15" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
+      <c r="C14" s="21"/>
+    </row>
+    <row r="15" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="72"/>
       <c r="B15" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="72"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="71"/>
+      <c r="C15" s="21"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="72"/>
       <c r="B16" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C16" s="72"/>
+      <c r="C16" s="21"/>
     </row>
     <row r="17" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="73"/>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C17" s="74"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="67"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="67"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="67"/>
+      <c r="C17" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>